<commit_message>
Added support for hidden pages to fix #9 Fixed NPE #8
</commit_message>
<xml_diff>
--- a/src/test/resources/org/concordion/ext/excel/HiddenColumn.xlsx
+++ b/src/test/resources/org/concordion/ext/excel/HiddenColumn.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="HiddenSheet" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -127,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Check the formatting</t>
   </si>
@@ -151,6 +152,9 @@
   </si>
   <si>
     <t>Some Hidden Row</t>
+  </si>
+  <si>
+    <t>This sheet is hidden, and shouldn't appear in the output.</t>
   </si>
 </sst>
 </file>
@@ -858,4 +862,29 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>